<commit_message>
add tpu results by different lr
</commit_message>
<xml_diff>
--- a/contest1_result/MeetTest_ScoreSheet.xlsx
+++ b/contest1_result/MeetTest_ScoreSheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
   <si>
     <t xml:space="preserve">model, runtime</t>
   </si>
@@ -153,7 +153,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -180,8 +180,11 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -202,8 +205,12 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
@@ -211,6 +218,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Accent 3 1" xfId="20"/>
+    <cellStyle name="Accent 3" xfId="21"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -283,7 +291,7 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -795,6 +803,46 @@
       </c>
       <c r="F31" s="0" t="n">
         <v>0.8832</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C32" s="3" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>0.871</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C33" s="3" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>0.8559</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>